<commit_message>
Found outliers in whole data set and took suspected outlier/s out. The model with only 1 outlier with the highest cooks distance was the best fit.
</commit_message>
<xml_diff>
--- a/Data/Larvae/R_larvae_resp_size.xlsx
+++ b/Data/Larvae/R_larvae_resp_size.xlsx
@@ -1,79 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nina Bean\Documents\Projects\Metabolic_scaling\Data\Larvae\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D391BF8-F376-4DFB-8862-7704E4BCEDE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="310" yWindow="0" windowWidth="18820" windowHeight="9160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>pikomol.larva.min</t>
-  </si>
-  <si>
-    <t>volume_mean.mm3</t>
-  </si>
-  <si>
-    <t>volume_se.mm3</t>
-  </si>
-  <si>
-    <t>log_resp</t>
-  </si>
-  <si>
-    <t>log_volume.mm3</t>
-  </si>
-  <si>
-    <t>#Date: 10/26/2020</t>
-  </si>
-  <si>
-    <t>#Temp: 26.7C</t>
-  </si>
-  <si>
-    <t>#Genotype: E</t>
-  </si>
-  <si>
-    <t>#Number of larvae: 6</t>
-  </si>
-  <si>
-    <t>#Volume: 2 mL</t>
-  </si>
-  <si>
-    <t>#larvae as spheroid (aka ellipsoid) = π/6*max length*max width^2 (Van Moorsel 1983)</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,14 +63,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -175,7 +109,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,27 +141,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,24 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -452,429 +350,439 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pikomol.larva.min</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>volume_mean.mm3</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>volume_se.mm3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Dry_weight.mg</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Dry_weight.mg.SE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>c_divide_SE.mg</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>46.801083304422143</v>
+        <v>46.85928571428569</v>
       </c>
       <c r="C2">
-        <v>0.15435278427333329</v>
+        <v>0.1543527842733333</v>
       </c>
       <c r="D2">
-        <v>2.803834340401086E-2</v>
+        <v>0.02803834340401086</v>
       </c>
       <c r="E2">
-        <v>1.6702559058024939</v>
+        <v>0.03158057966232399</v>
       </c>
       <c r="F2">
-        <v>-0.81148553214470565</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.005736645060460621</v>
+      </c>
+      <c r="G2">
+        <v>0.07883655027428632</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>94.765859042553217</v>
+        <v>142.073625</v>
       </c>
       <c r="C3">
-        <v>0.32565413302666668</v>
+        <v>0.3256541330266667</v>
       </c>
       <c r="D3">
-        <v>2.0849036915702938E-2</v>
+        <v>0.02084903691570294</v>
       </c>
       <c r="E3">
-        <v>1.9766519037939541</v>
+        <v>0.06662883561725601</v>
       </c>
       <c r="F3">
-        <v>-0.48724340562352508</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.00426571295295282</v>
+      </c>
+      <c r="G3">
+        <v>0.02778555867637069</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>88.974277017859123</v>
+        <v>88.97427701785912</v>
       </c>
       <c r="C4">
-        <v>0.23187812408666669</v>
+        <v>0.2318781240866667</v>
       </c>
       <c r="D4">
-        <v>2.452890689928065E-2</v>
+        <v>0.02452890689928065</v>
       </c>
       <c r="E4">
-        <v>1.949264467724718</v>
+        <v>0.047442264188132</v>
       </c>
       <c r="F4">
-        <v>-0.63474022176557798</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.005018614351592821</v>
+      </c>
+      <c r="G4">
+        <v>0.04591009020889322</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>61.163697590136422</v>
+        <v>61.22189999999998</v>
       </c>
       <c r="C5">
-        <v>0.32961901983611108</v>
+        <v>0.3296190198361111</v>
       </c>
       <c r="D5">
-        <v>7.5558585564302921E-2</v>
+        <v>0.07555858556430292</v>
       </c>
       <c r="E5">
-        <v>1.7864937323722609</v>
+        <v>0.06744005145846832</v>
       </c>
       <c r="F5">
-        <v>-0.4819877363816335</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.01545928660645638</v>
+      </c>
+      <c r="G5">
+        <v>0.09948584323566066</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6">
         <v>9</v>
       </c>
       <c r="B6">
-        <v>44.193080711103342</v>
+        <v>57.91361344537825</v>
       </c>
       <c r="C6">
-        <v>0.16777398727611109</v>
+        <v>0.1677739872761111</v>
       </c>
       <c r="D6">
-        <v>2.199873199457144E-2</v>
+        <v>0.02199873199457144</v>
       </c>
       <c r="E6">
-        <v>1.6453542773983989</v>
+        <v>0.03432655779669232</v>
       </c>
       <c r="F6">
-        <v>-0.77527537400905711</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.004500940566089316</v>
+      </c>
+      <c r="G6">
+        <v>0.0569066149088503</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>52.457374513213367</v>
+        <v>52.51557692307694</v>
       </c>
       <c r="C7">
-        <v>0.24116995452000001</v>
+        <v>0.24116995452</v>
       </c>
       <c r="D7">
-        <v>3.9730413528174288E-2</v>
+        <v>0.03973041352817429</v>
       </c>
       <c r="E7">
-        <v>1.719806550399253</v>
+        <v>0.049343372694792</v>
       </c>
       <c r="F7">
-        <v>-0.61767679851757074</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.008128842607864459</v>
+      </c>
+      <c r="G7">
+        <v>0.07149729536395337</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8">
         <v>19</v>
       </c>
       <c r="B8">
-        <v>67.475621111879036</v>
+        <v>81.19615384615396</v>
       </c>
       <c r="C8">
-        <v>0.37243690257722217</v>
+        <v>0.3724369025772222</v>
       </c>
       <c r="D8">
-        <v>7.0772128714042148E-2</v>
+        <v>0.07077212871404215</v>
       </c>
       <c r="E8">
-        <v>1.8291468909198501</v>
+        <v>0.07620059026729967</v>
       </c>
       <c r="F8">
-        <v>-0.42894729387855901</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.01447997753489302</v>
+      </c>
+      <c r="G8">
+        <v>0.08247062428386973</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9">
         <v>20</v>
       </c>
       <c r="B9">
-        <v>84.18532227784722</v>
+        <v>131.493088235294</v>
       </c>
       <c r="C9">
-        <v>0.34709090910166668</v>
+        <v>0.3470909091016667</v>
       </c>
       <c r="D9">
-        <v>1.7836853327042129E-2</v>
+        <v>0.01783685332704213</v>
       </c>
       <c r="E9">
-        <v>1.925236378798949</v>
+        <v>0.07101480000220099</v>
       </c>
       <c r="F9">
-        <v>-0.45955676108711668</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.003649420190712819</v>
+      </c>
+      <c r="G9">
+        <v>0.02230307432704556</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10">
         <v>23</v>
       </c>
       <c r="B10">
-        <v>77.038494837842791</v>
+        <v>77.09669724770636</v>
       </c>
       <c r="C10">
-        <v>0.35353293775933331</v>
+        <v>0.3535329377593333</v>
       </c>
       <c r="D10">
-        <v>4.942376071159979E-2</v>
+        <v>0.04942376071159979</v>
       </c>
       <c r="E10">
-        <v>1.886707789043724</v>
+        <v>0.07233283906555958</v>
       </c>
       <c r="F10">
-        <v>-0.45157011787630819</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.01011210144159332</v>
+      </c>
+      <c r="G10">
+        <v>0.06067302324016069</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11">
         <v>26</v>
       </c>
       <c r="B11">
-        <v>75.755300599058444</v>
+        <v>89.47583333333337</v>
       </c>
       <c r="C11">
-        <v>0.21954213037833331</v>
+        <v>0.2195421303783333</v>
       </c>
       <c r="D11">
-        <v>2.4780536715410782E-2</v>
+        <v>0.02478053671541078</v>
       </c>
       <c r="E11">
-        <v>1.879413025826274</v>
+        <v>0.044918319875407</v>
       </c>
       <c r="F11">
-        <v>-0.65848212583137267</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.005070097811973045</v>
+      </c>
+      <c r="G11">
+        <v>0.04898719401125783</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12">
         <v>30</v>
       </c>
       <c r="B12">
-        <v>39.813633932391816</v>
+        <v>53.53416666666674</v>
       </c>
       <c r="C12">
-        <v>0.10646527881499999</v>
+        <v>0.106465278815</v>
       </c>
       <c r="D12">
-        <v>1.8743670660645761E-2</v>
+        <v>0.01874367066064576</v>
       </c>
       <c r="E12">
-        <v>1.6000318189998071</v>
+        <v>0.021782796045549</v>
       </c>
       <c r="F12">
-        <v>-0.97279200422197976</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.003834955017168123</v>
+      </c>
+      <c r="G12">
+        <v>0.07640756833836562</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13">
         <v>31</v>
       </c>
       <c r="B13">
-        <v>62.853998748435622</v>
+        <v>110.1617647058824</v>
       </c>
       <c r="C13">
-        <v>0.47122128897055549</v>
+        <v>0.4712212889705555</v>
       </c>
       <c r="D13">
         <v>0.1008814728620932</v>
       </c>
       <c r="E13">
-        <v>1.7983329125571701</v>
+        <v>0.09641187572337566</v>
       </c>
       <c r="F13">
-        <v>-0.3267750970970531</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.02064034934758426</v>
+      </c>
+      <c r="G13">
+        <v>0.09291294821971467</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14">
         <v>33</v>
       </c>
       <c r="B14">
-        <v>81.930173177176258</v>
+        <v>81.93017317717626</v>
       </c>
       <c r="C14">
-        <v>0.26511452081444442</v>
+        <v>0.2651145208144444</v>
       </c>
       <c r="D14">
-        <v>2.3349481348405969E-2</v>
+        <v>0.02334948134840597</v>
       </c>
       <c r="E14">
-        <v>1.91344387283587</v>
+        <v>0.05424243095863533</v>
       </c>
       <c r="F14">
-        <v>-0.57656648450048387</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.004777303883883861</v>
+      </c>
+      <c r="G14">
+        <v>0.0382237641079676</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15">
         <v>35</v>
       </c>
       <c r="B15">
-        <v>74.059937125020156</v>
+        <v>74.11813953488371</v>
       </c>
       <c r="C15">
-        <v>0.42511677747499999</v>
+        <v>0.425116777475</v>
       </c>
       <c r="D15">
-        <v>3.6956360678030258E-2</v>
+        <v>0.03695636067803026</v>
       </c>
       <c r="E15">
-        <v>1.8695833390087471</v>
+        <v>0.08697889267138499</v>
       </c>
       <c r="F15">
-        <v>-0.37149175501633852</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.007561271394724992</v>
+      </c>
+      <c r="G15">
+        <v>0.03772859925578531</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16">
         <v>40</v>
       </c>
       <c r="B16">
-        <v>73.470602910602977</v>
+        <v>77.70384615384631</v>
       </c>
       <c r="C16">
         <v>0.2162281759483333</v>
       </c>
       <c r="D16">
-        <v>1.559647306622867E-2</v>
+        <v>0.01559647306622867</v>
       </c>
       <c r="E16">
-        <v>1.8661136037435679</v>
+        <v>0.044240284799029</v>
       </c>
       <c r="F16">
-        <v>-0.66508771527821953</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.003191038389350386</v>
+      </c>
+      <c r="G16">
+        <v>0.03130428900422594</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17">
         <v>43</v>
       </c>
       <c r="B17">
-        <v>73.013423309681244</v>
+        <v>86.73395604395616</v>
       </c>
       <c r="C17">
         <v>0.2902047782983333</v>
       </c>
       <c r="D17">
-        <v>2.1095528799829719E-2</v>
+        <v>0.02109552879982972</v>
       </c>
       <c r="E17">
-        <v>1.863402711263012</v>
+        <v>0.059375897639839</v>
       </c>
       <c r="F17">
-        <v>-0.53729544106604765</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.00431614519244516</v>
+      </c>
+      <c r="G17">
+        <v>0.03154827275005857</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18">
         <v>47</v>
       </c>
       <c r="B18">
-        <v>84.026380923469802</v>
+        <v>84.08458333333336</v>
       </c>
       <c r="C18">
-        <v>0.31567474446888888</v>
+        <v>0.3156747444688889</v>
       </c>
       <c r="D18">
-        <v>1.9803456792886979E-2</v>
+        <v>0.01980345679288698</v>
       </c>
       <c r="E18">
-        <v>1.924415658571027</v>
+        <v>0.06458705271833466</v>
       </c>
       <c r="F18">
-        <v>-0.50076016241107013</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12E1628-0F34-4287-B722-D24C7E7B919F}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="73.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>11</v>
+        <v>0.004051787259824676</v>
+      </c>
+      <c r="G18">
+        <v>0.02722644240220489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>